<commit_message>
Excel actualizado de nuevo
</commit_message>
<xml_diff>
--- a/files/results.xlsx
+++ b/files/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Gits\Digievolucion\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71BF06C-EE80-42F4-8605-666139BC3E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD5184-1396-47FC-967F-79B7AABBB0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>chromosomeJorge1</t>
   </si>
@@ -151,6 +151,24 @@
   </si>
   <si>
     <t>{1, 3, 6, 8, 10, 14}</t>
+  </si>
+  <si>
+    <t>chromosomeRaul</t>
+  </si>
+  <si>
+    <t>chromosomeRaul2</t>
+  </si>
+  <si>
+    <t>chromosomeCarlos15_3</t>
+  </si>
+  <si>
+    <t>chromosomeMPL</t>
+  </si>
+  <si>
+    <t>chromosomeCarlos15_4</t>
+  </si>
+  <si>
+    <t>{1, 2, 6, 7, 8, 9, 11, 13}</t>
   </si>
 </sst>
 </file>
@@ -329,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,11 +376,377 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -447,370 +831,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -922,9 +942,1684 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Comparación</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" baseline="0"/>
+              <a:t> Fitness 1+1</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>base</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$Q$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>251.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>153.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>172.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>446.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>131.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>479.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>325.45999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>376.73</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>369.57</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>525.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>333.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>462.78600000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001C-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chromosomeCarlos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Map 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Map 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Map 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Map 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Map 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Map 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Map 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Map 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Map 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Map 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Map 11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Map 12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Map 13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Map 14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$Q$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>279.94</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>158.13999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>343.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>166.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>295.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>374.86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>395.68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>417.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>417.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>285.12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>377.83</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>281.98</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>311.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>317.59866666666665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chromosomeCarlos15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Map 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Map 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Map 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Map 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Map 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Map 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Map 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Map 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Map 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Map 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Map 11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Map 12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Map 13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Map 14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>179.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>189.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>173.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>382.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179.73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>464.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>303.81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>418.71</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>351.66</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>386.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>296.94</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>325.74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>236.58</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>324.33</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>304.32799999999992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chromosomeCarlos2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Map 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Map 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Map 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Map 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Map 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Map 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Map 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Map 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Map 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Map 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Map 11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Map 12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Map 13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Map 14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>211.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>194.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>196.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>365.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>138.49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>448.84</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>278.43</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>338.31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>414.09</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>354.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>426.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>297.77999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>357.68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>235.77</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>317.27999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>304.98399999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chromosomeCarlos15_2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Map 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Map 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Map 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Map 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Map 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Map 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Map 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Map 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Map 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Map 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Map 11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Map 12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Map 13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Map 14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>166.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>328.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>143.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>484.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>261.08999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>330.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>378.88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>330.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>447.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>304.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>357.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>277.07</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>310.44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>296.98199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>chromosomeJorge2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>Map 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Map 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Map 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Map 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Map 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Map 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Map 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Map 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Map 9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Map 10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Map 11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Map 12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Map 13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Map 14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>159.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>169.64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191.31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>381.59</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>132.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>482.22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>264.29000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>343.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>353.63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>302.64999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>382.46</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>343.86</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>327.12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248.38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>305.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>292.54000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7497-45FA-9476-A33BFAF74754}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="545364400"/>
+        <c:axId val="545344016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="545364400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545344016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="545344016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545364400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>153458</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>156634</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>467783</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>166158</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75CA5D8-B1E4-426B-A560-074200025C77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}" name="Table1" displayName="Table1" ref="A2:Q16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A2:Q16" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}" name="Table1" displayName="Table1" ref="A2:Q21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A2:Q21" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -945,22 +2640,22 @@
   </autoFilter>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{83342CD1-3207-424D-BF4E-5884CA5C5C5A}" name="Model" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{F73BD6E6-80F1-4E55-A37D-A2B257F74134}" name="Map 0" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2F7B3B44-6101-4CD9-849C-C445B532E80D}" name="Map 1" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0E3F57E6-AC19-4812-BA3C-007211C76514}" name="Map 2" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{37139713-BDCE-49D8-9FC1-641524B486E6}" name="Map 3" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{D024F6F3-0F24-4674-882F-D83DD1138804}" name="Map 4" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{74446B40-6A27-4FD6-8AF1-C282182D48E5}" name="Map 5" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{9BADCBF4-A1B2-4D01-B4C4-FF537BDF38BE}" name="Map 6" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{46C3F92D-D9B4-41FD-BB07-0E2C0946E73D}" name="Map 7" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{2B32E458-3379-4DB3-907F-9B4531E69142}" name="Map 8" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{3C93BE20-B93F-4F49-80EB-93CD30F87DC3}" name="Map 9" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{71477164-69AD-4967-8E8B-D1162DD1148F}" name="Map 10" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{BCEDDECE-BF9C-40A3-BFE6-27514C89EBD1}" name="Map 11" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{52D0F212-A73F-4F9A-A7FD-DB408A2494CE}" name="Map 12" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{33536C40-8D2A-453D-AB8D-6E002F262075}" name="Map 13" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{3B1FC886-981A-40F4-8C66-EE4A4151FD4A}" name="Map 14" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{020A042A-A175-4E96-A7B8-C7E12C90CBD0}" name="Average" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{F73BD6E6-80F1-4E55-A37D-A2B257F74134}" name="Map 0" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{2F7B3B44-6101-4CD9-849C-C445B532E80D}" name="Map 1" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{0E3F57E6-AC19-4812-BA3C-007211C76514}" name="Map 2" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{37139713-BDCE-49D8-9FC1-641524B486E6}" name="Map 3" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{D024F6F3-0F24-4674-882F-D83DD1138804}" name="Map 4" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{74446B40-6A27-4FD6-8AF1-C282182D48E5}" name="Map 5" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{9BADCBF4-A1B2-4D01-B4C4-FF537BDF38BE}" name="Map 6" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{46C3F92D-D9B4-41FD-BB07-0E2C0946E73D}" name="Map 7" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{2B32E458-3379-4DB3-907F-9B4531E69142}" name="Map 8" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{3C93BE20-B93F-4F49-80EB-93CD30F87DC3}" name="Map 9" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{71477164-69AD-4967-8E8B-D1162DD1148F}" name="Map 10" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{BCEDDECE-BF9C-40A3-BFE6-27514C89EBD1}" name="Map 11" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{52D0F212-A73F-4F9A-A7FD-DB408A2494CE}" name="Map 12" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{33536C40-8D2A-453D-AB8D-6E002F262075}" name="Map 13" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{3B1FC886-981A-40F4-8C66-EE4A4151FD4A}" name="Map 14" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{020A042A-A175-4E96-A7B8-C7E12C90CBD0}" name="Average" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1231,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T16"/>
+  <dimension ref="A2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,64 +3739,345 @@
         <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
         <v>304.32799999999992</v>
       </c>
+      <c r="S15" s="6"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="12">
         <v>166.91</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="12">
         <v>167.92</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="12">
         <v>164.55</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="12">
         <v>328.63</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="12">
         <v>143.74</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="12">
         <v>484.96</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="12">
         <v>261.08999999999997</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="12">
         <v>330.21</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="12">
         <v>378.88</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="12">
         <v>330.9</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="12">
         <v>447.99</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="12">
         <v>304.32</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="12">
         <v>357.12</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="12">
         <v>277.07</v>
       </c>
-      <c r="P16" s="6">
+      <c r="P16" s="12">
         <v>310.44</v>
       </c>
       <c r="Q16" s="11">
         <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
         <v>296.98199999999997</v>
       </c>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13">
+        <v>165.77</v>
+      </c>
+      <c r="C17" s="13">
+        <v>169.48</v>
+      </c>
+      <c r="D17" s="13">
+        <v>156.93</v>
+      </c>
+      <c r="E17" s="13">
+        <v>475.34</v>
+      </c>
+      <c r="F17" s="13">
+        <v>154.58000000000001</v>
+      </c>
+      <c r="G17" s="13">
+        <v>443.05</v>
+      </c>
+      <c r="H17" s="13">
+        <v>266.08999999999997</v>
+      </c>
+      <c r="I17" s="13">
+        <v>333.29</v>
+      </c>
+      <c r="J17" s="13">
+        <v>339.92</v>
+      </c>
+      <c r="K17" s="13">
+        <v>364.88</v>
+      </c>
+      <c r="L17" s="13">
+        <v>435.58</v>
+      </c>
+      <c r="M17" s="13">
+        <v>337.48</v>
+      </c>
+      <c r="N17" s="13">
+        <v>513.04999999999995</v>
+      </c>
+      <c r="O17" s="13">
+        <v>345.37</v>
+      </c>
+      <c r="P17" s="13">
+        <v>296.2</v>
+      </c>
+      <c r="Q17" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
+        <v>319.80066666666664</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13">
+        <v>228.8</v>
+      </c>
+      <c r="C18" s="13">
+        <v>207.67</v>
+      </c>
+      <c r="D18" s="13">
+        <v>187.5</v>
+      </c>
+      <c r="E18" s="13">
+        <v>405.93</v>
+      </c>
+      <c r="F18" s="13">
+        <v>180.39</v>
+      </c>
+      <c r="G18" s="13">
+        <v>585.16</v>
+      </c>
+      <c r="H18" s="13">
+        <v>250.9</v>
+      </c>
+      <c r="I18" s="13">
+        <v>362.43</v>
+      </c>
+      <c r="J18" s="13">
+        <v>388.74</v>
+      </c>
+      <c r="K18" s="13">
+        <v>350.02</v>
+      </c>
+      <c r="L18" s="13">
+        <v>573.97</v>
+      </c>
+      <c r="M18" s="13">
+        <v>330.8</v>
+      </c>
+      <c r="N18" s="13">
+        <v>411.47</v>
+      </c>
+      <c r="O18" s="13">
+        <v>315.67</v>
+      </c>
+      <c r="P18" s="13">
+        <v>318.35000000000002</v>
+      </c>
+      <c r="Q18" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
+        <v>339.85333333333335</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="13">
+        <v>177.69</v>
+      </c>
+      <c r="C19" s="13">
+        <v>158.79</v>
+      </c>
+      <c r="D19" s="13">
+        <v>173.24</v>
+      </c>
+      <c r="E19" s="13">
+        <v>413.66</v>
+      </c>
+      <c r="F19" s="13">
+        <v>157.99</v>
+      </c>
+      <c r="G19" s="13">
+        <v>456.55</v>
+      </c>
+      <c r="H19" s="13">
+        <v>291.43</v>
+      </c>
+      <c r="I19" s="13">
+        <v>322.97000000000003</v>
+      </c>
+      <c r="J19" s="13">
+        <v>372.77</v>
+      </c>
+      <c r="K19" s="13">
+        <v>351.88</v>
+      </c>
+      <c r="L19" s="13">
+        <v>414.53</v>
+      </c>
+      <c r="M19" s="13">
+        <v>346.99</v>
+      </c>
+      <c r="N19" s="13">
+        <v>371.46</v>
+      </c>
+      <c r="O19" s="13">
+        <v>234.89</v>
+      </c>
+      <c r="P19" s="13">
+        <v>291.52</v>
+      </c>
+      <c r="Q19" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
+        <v>302.42400000000004</v>
+      </c>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="13">
+        <v>159.25</v>
+      </c>
+      <c r="C20" s="13">
+        <v>169.64</v>
+      </c>
+      <c r="D20" s="13">
+        <v>191.31</v>
+      </c>
+      <c r="E20" s="13">
+        <v>381.59</v>
+      </c>
+      <c r="F20" s="13">
+        <v>132.82</v>
+      </c>
+      <c r="G20" s="13">
+        <v>482.22</v>
+      </c>
+      <c r="H20" s="13">
+        <v>264.29000000000002</v>
+      </c>
+      <c r="I20" s="13">
+        <v>343.38</v>
+      </c>
+      <c r="J20" s="13">
+        <v>353.63</v>
+      </c>
+      <c r="K20" s="13">
+        <v>302.64999999999998</v>
+      </c>
+      <c r="L20" s="13">
+        <v>382.46</v>
+      </c>
+      <c r="M20" s="13">
+        <v>343.86</v>
+      </c>
+      <c r="N20" s="13">
+        <v>327.12</v>
+      </c>
+      <c r="O20" s="13">
+        <v>248.38</v>
+      </c>
+      <c r="P20" s="13">
+        <v>305.5</v>
+      </c>
+      <c r="Q20" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
+        <v>292.54000000000002</v>
+      </c>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="13">
+        <v>272.79000000000002</v>
+      </c>
+      <c r="C21" s="13">
+        <v>190.29</v>
+      </c>
+      <c r="D21" s="13">
+        <v>249.96</v>
+      </c>
+      <c r="E21" s="13">
+        <v>431.17</v>
+      </c>
+      <c r="F21" s="13">
+        <v>148.75</v>
+      </c>
+      <c r="G21" s="13">
+        <v>586.79</v>
+      </c>
+      <c r="H21" s="13">
+        <v>273.98</v>
+      </c>
+      <c r="I21" s="13">
+        <v>319.3</v>
+      </c>
+      <c r="J21" s="13">
+        <v>377.47</v>
+      </c>
+      <c r="K21" s="13">
+        <v>374.58</v>
+      </c>
+      <c r="L21" s="13">
+        <v>354.47</v>
+      </c>
+      <c r="M21" s="13">
+        <v>317.05</v>
+      </c>
+      <c r="N21" s="13">
+        <v>484.09</v>
+      </c>
+      <c r="O21" s="13">
+        <v>287.8</v>
+      </c>
+      <c r="P21" s="13">
+        <v>326.98</v>
+      </c>
+      <c r="Q21" s="11">
+        <f>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</f>
+        <v>333.03133333333341</v>
+      </c>
+      <c r="S21" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C16">
+  <conditionalFormatting sqref="C3:C21">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2113,7 +4089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E16">
+  <conditionalFormatting sqref="E3:E21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2125,7 +4101,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B16">
+  <conditionalFormatting sqref="B3:B21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2137,7 +4113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D16">
+  <conditionalFormatting sqref="D3:D21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2149,7 +4125,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F16">
+  <conditionalFormatting sqref="F3:F21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2161,7 +4137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G16">
+  <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2173,7 +4149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H16">
+  <conditionalFormatting sqref="H3:H21">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2185,7 +4161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I16">
+  <conditionalFormatting sqref="I3:I21">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2197,7 +4173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J16">
+  <conditionalFormatting sqref="J3:J21">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2209,7 +4185,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K16">
+  <conditionalFormatting sqref="K3:K21">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2221,7 +4197,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L16">
+  <conditionalFormatting sqref="L3:L21">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2233,7 +4209,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M16">
+  <conditionalFormatting sqref="M3:M21">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2245,7 +4221,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N16">
+  <conditionalFormatting sqref="N3:N21">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2257,7 +4233,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O16">
+  <conditionalFormatting sqref="O3:O21">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -2269,7 +4245,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P16">
+  <conditionalFormatting sqref="P3:P21">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -2281,7 +4257,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q16">
+  <conditionalFormatting sqref="Q3:Q21">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -2294,8 +4270,10 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Datos de dos mapas de Carlos
</commit_message>
<xml_diff>
--- a/files/results.xlsx
+++ b/files/results.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Gits\Digievolucion\files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD5184-1396-47FC-967F-79B7AABBB0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>chromosomeJorge1</t>
   </si>
@@ -169,12 +163,24 @@
   </si>
   <si>
     <t>{1, 2, 6, 7, 8, 9, 11, 13}</t>
+  </si>
+  <si>
+    <t>Ciclo</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>chromosomeCarlos3</t>
+  </si>
+  <si>
+    <t>chromosomeCarlos4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +216,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +227,12 @@
       <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -347,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,6 +390,21 @@
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +418,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -417,7 +443,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -447,7 +472,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -475,7 +499,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -503,7 +526,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -531,7 +553,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -559,7 +580,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -587,7 +607,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -615,7 +634,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -643,7 +661,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -671,7 +688,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -699,7 +715,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -727,7 +742,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -755,7 +769,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -783,7 +796,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -811,7 +823,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -841,7 +852,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -889,7 +899,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -914,7 +923,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -943,9 +951,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -987,6 +995,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -995,26 +1004,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1104,7 +1093,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001C-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1247,7 +1236,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1390,7 +1379,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1533,7 +1522,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1676,7 +1665,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1819,7 +1808,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7497-45FA-9476-A33BFAF74754}"/>
             </c:ext>
@@ -1834,11 +1823,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="545364400"/>
-        <c:axId val="545344016"/>
+        <c:axId val="200990208"/>
+        <c:axId val="134798080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="545364400"/>
+        <c:axId val="200990208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,7 +1870,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545344016"/>
+        <c:crossAx val="134798080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1889,7 +1878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="545344016"/>
+        <c:axId val="134798080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1929,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="545364400"/>
+        <c:crossAx val="200990208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1954,6 +1943,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2020,562 +2010,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2596,7 +2030,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75CA5D8-B1E4-426B-A560-074200025C77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E75CA5D8-B1E4-426B-A560-074200025C77}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2618,8 +2052,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}" name="Table1" displayName="Table1" ref="A2:Q21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A2:Q21" xr:uid="{FE955E96-146C-4D29-9D73-640EF3E1413E}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:Q21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="A2:Q21">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2639,23 +2073,23 @@
     <filterColumn colId="16" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{83342CD1-3207-424D-BF4E-5884CA5C5C5A}" name="Model" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{F73BD6E6-80F1-4E55-A37D-A2B257F74134}" name="Map 0" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{2F7B3B44-6101-4CD9-849C-C445B532E80D}" name="Map 1" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{0E3F57E6-AC19-4812-BA3C-007211C76514}" name="Map 2" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{37139713-BDCE-49D8-9FC1-641524B486E6}" name="Map 3" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{D024F6F3-0F24-4674-882F-D83DD1138804}" name="Map 4" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{74446B40-6A27-4FD6-8AF1-C282182D48E5}" name="Map 5" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{9BADCBF4-A1B2-4D01-B4C4-FF537BDF38BE}" name="Map 6" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{46C3F92D-D9B4-41FD-BB07-0E2C0946E73D}" name="Map 7" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{2B32E458-3379-4DB3-907F-9B4531E69142}" name="Map 8" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{3C93BE20-B93F-4F49-80EB-93CD30F87DC3}" name="Map 9" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{71477164-69AD-4967-8E8B-D1162DD1148F}" name="Map 10" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{BCEDDECE-BF9C-40A3-BFE6-27514C89EBD1}" name="Map 11" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{52D0F212-A73F-4F9A-A7FD-DB408A2494CE}" name="Map 12" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{33536C40-8D2A-453D-AB8D-6E002F262075}" name="Map 13" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{3B1FC886-981A-40F4-8C66-EE4A4151FD4A}" name="Map 14" dataDxfId="1"/>
-    <tableColumn id="17" xr3:uid="{020A042A-A175-4E96-A7B8-C7E12C90CBD0}" name="Average" dataDxfId="0">
+    <tableColumn id="1" name="Model" dataDxfId="16"/>
+    <tableColumn id="2" name="Map 0" dataDxfId="15"/>
+    <tableColumn id="3" name="Map 1" dataDxfId="14"/>
+    <tableColumn id="4" name="Map 2" dataDxfId="13"/>
+    <tableColumn id="5" name="Map 3" dataDxfId="12"/>
+    <tableColumn id="6" name="Map 4" dataDxfId="11"/>
+    <tableColumn id="7" name="Map 5" dataDxfId="10"/>
+    <tableColumn id="8" name="Map 6" dataDxfId="9"/>
+    <tableColumn id="9" name="Map 7" dataDxfId="8"/>
+    <tableColumn id="10" name="Map 8" dataDxfId="7"/>
+    <tableColumn id="11" name="Map 9" dataDxfId="6"/>
+    <tableColumn id="12" name="Map 10" dataDxfId="5"/>
+    <tableColumn id="13" name="Map 11" dataDxfId="4"/>
+    <tableColumn id="14" name="Map 12" dataDxfId="3"/>
+    <tableColumn id="15" name="Map 13" dataDxfId="2"/>
+    <tableColumn id="16" name="Map 14" dataDxfId="1"/>
+    <tableColumn id="17" name="Average" dataDxfId="0">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[Map 0]:[Map 14]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2706,7 +2140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2741,7 +2175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2918,28 +2352,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:T21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="9.7109375" customWidth="1"/>
-    <col min="19" max="19" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="9.7265625" customWidth="1"/>
+    <col min="19" max="19" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="34" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
@@ -2997,7 +2434,7 @@
       </c>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -3054,7 +2491,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -3111,7 +2548,7 @@
       <c r="S4" s="6"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -3168,7 +2605,7 @@
       <c r="S5" s="6"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -3226,8 +2663,50 @@
         <v>26</v>
       </c>
       <c r="T6" s="4"/>
+      <c r="U6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="14">
+        <v>1</v>
+      </c>
+      <c r="X6" s="14">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="14">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="14">
+        <v>12</v>
+      </c>
+      <c r="AA6" s="14">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="14">
+        <v>45</v>
+      </c>
+      <c r="AC6" s="14">
+        <v>78</v>
+      </c>
+      <c r="AD6" s="14">
+        <v>82</v>
+      </c>
+      <c r="AE6" s="14">
+        <v>137</v>
+      </c>
+      <c r="AF6" s="14">
+        <v>152</v>
+      </c>
+      <c r="AG6" s="14">
+        <v>165</v>
+      </c>
+      <c r="AH6" s="18">
+        <v>194</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -3284,8 +2763,48 @@
         <v>28</v>
       </c>
       <c r="T7" s="4"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7" s="14">
+        <v>325.56</v>
+      </c>
+      <c r="X7" s="14">
+        <v>323.77</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>292.81</v>
+      </c>
+      <c r="Z7" s="14">
+        <v>291.55</v>
+      </c>
+      <c r="AA7" s="14">
+        <v>280.76</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>274.67</v>
+      </c>
+      <c r="AC7" s="14">
+        <v>270.58999999999997</v>
+      </c>
+      <c r="AD7" s="14">
+        <v>246.75</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>241.08</v>
+      </c>
+      <c r="AF7" s="14">
+        <v>237.06</v>
+      </c>
+      <c r="AG7" s="14">
+        <v>234.19</v>
+      </c>
+      <c r="AH7" s="18">
+        <v>231.78</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -3342,8 +2861,38 @@
         <v>24</v>
       </c>
       <c r="T8" s="4"/>
+      <c r="U8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="14">
+        <v>0</v>
+      </c>
+      <c r="X8" s="14">
+        <v>4</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="14">
+        <v>23</v>
+      </c>
+      <c r="AA8" s="14">
+        <v>32</v>
+      </c>
+      <c r="AB8" s="14">
+        <v>57</v>
+      </c>
+      <c r="AC8" s="14">
+        <v>79</v>
+      </c>
+      <c r="AD8" s="14">
+        <v>157</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>3</v>
       </c>
@@ -3400,8 +2949,36 @@
         <v>27</v>
       </c>
       <c r="T9" s="4"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" s="14">
+        <v>359.62</v>
+      </c>
+      <c r="X9" s="14">
+        <v>303.95999999999998</v>
+      </c>
+      <c r="Y9" s="14">
+        <v>261.77</v>
+      </c>
+      <c r="Z9" s="14">
+        <v>252.05</v>
+      </c>
+      <c r="AA9" s="14">
+        <v>247.84</v>
+      </c>
+      <c r="AB9" s="14">
+        <v>238</v>
+      </c>
+      <c r="AC9" s="14">
+        <v>230.84</v>
+      </c>
+      <c r="AD9" s="14">
+        <v>227.91</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
@@ -3458,7 +3035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
@@ -3515,7 +3092,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
@@ -3572,7 +3149,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>32</v>
       </c>
@@ -3629,7 +3206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -3686,7 +3263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -3741,7 +3318,7 @@
       </c>
       <c r="S15" s="6"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
@@ -3796,7 +3373,7 @@
       </c>
       <c r="S16" s="6"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>39</v>
       </c>
@@ -3853,7 +3430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
@@ -3910,7 +3487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>41</v>
       </c>
@@ -3965,7 +3542,7 @@
       </c>
       <c r="S19" s="6"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
@@ -4020,7 +3597,7 @@
       </c>
       <c r="S20" s="6"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>43</v>
       </c>
@@ -4076,6 +3653,10 @@
       <c r="S21" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="U8:U9"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C3:C21">
     <cfRule type="colorScale" priority="2">

</xml_diff>